<commit_message>
aggiornamento checklist.xlsx, data.json e file pdf in FILES folder
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8A5219-DD3A-4D24-BAB7-D75D69AD7429}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC83D705-0093-43A8-B712-22428ED0D7B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="8850" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="908">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4543,64 +4543,16 @@
     <t>subject_application_version: 7</t>
   </si>
   <si>
-    <t>2023-10-23T12:52:39Z</t>
-  </si>
-  <si>
-    <t>d4aa7beba8ac9bb3</t>
-  </si>
-  <si>
     <t>Messaggio errore</t>
   </si>
   <si>
     <t>Il PLS viene avvisato con l'errore mostrato a video e viene annullato l'invio del PS.</t>
   </si>
   <si>
-    <t>2023-10-23T14:34:13Z</t>
-  </si>
-  <si>
-    <t>b7185552b516032e</t>
-  </si>
-  <si>
     <t>Viene mostrato un errore a video contenente il messaggio "Impossibile contattare il servizio di validazione"</t>
   </si>
   <si>
     <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.</t>
-  </si>
-  <si>
-    <t>2023-10-24T15:25:46Z</t>
-  </si>
-  <si>
-    <t>fdfb77c1b2df0614</t>
-  </si>
-  <si>
-    <t>2023-10-24T15:48:30Z</t>
-  </si>
-  <si>
-    <t>f69cdfeca881af55</t>
-  </si>
-  <si>
-    <t>6685c330dc468a8c</t>
-  </si>
-  <si>
-    <t>2023-10-24T16:01:26Z</t>
-  </si>
-  <si>
-    <t>6390feab6bc73fd3</t>
-  </si>
-  <si>
-    <t>2023-10-24T16:11:15Z</t>
-  </si>
-  <si>
-    <t>da9bd7ee8ca1f994</t>
-  </si>
-  <si>
-    <t>2023-10-24T16:19:00Z</t>
-  </si>
-  <si>
-    <t>2023-10-24T16:29:04Z</t>
-  </si>
-  <si>
-    <t>5d59277bd078d917</t>
   </si>
   <si>
     <t>Essendo un elemento opzionale non viene costruito l'elemento XML.</t>
@@ -4646,79 +4598,130 @@
     <t>Essendo comunque una sezione obbligatoria, non c'è modo che il medico possa omettere questa sezione nel compilare il CDA</t>
   </si>
   <si>
-    <t>2023-10-25T10:07:07Z</t>
-  </si>
-  <si>
-    <t>1f590a215d4a5b94</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.f4f0b282c20e5dafefd9eb02f3ad6e1ef442d17cd16a0605232bc5a5bd95c417.1931bf3eef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-25T10:18:20Z</t>
-  </si>
-  <si>
-    <t>69219fae5ac703ee</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.6225c76e438eb1ba8d940db7939244f27b7b62b7c47619e1600cca02114d7c9d.b55fe31253^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-10-25T13:27:35Z</t>
-  </si>
-  <si>
-    <t>9115df9e4db55163</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.3395fa274808e71dab6b0b197e79ceba29acc2410c15555990285332770bbeaf.2bf2f65653^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Le sezioni Piani di cura e Visite/Ricoveri (opzionali) e Stile di vita (raccomandato) sono state omesse.
 In particolare Stile di vita, gestendo la cartella clinica solo bambini in età pediatrica, non prevede la compilazione dei campi contenuti in questa sezione.</t>
   </si>
   <si>
-    <t>2023-10-25T14:58:52Z</t>
-  </si>
-  <si>
-    <t>29a8c6fa752a61ad</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.de885a82ca264f6855821a9ad65f8605586ea746dbb16dc73c781ee94a2611d8.c62e11fb96^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Le sezioni Piani di cura e Visite/Ricoveri e Gravidanza e Parto (opzionali) e Stile di vita (raccomandato) sono state omesse.
 In particolare Stile di vita e Gravidanza e Parto, gestendo la cartella clinica solo bambini in età pediatrica, non prevede la compilazione dei campi contenuti in questa sezione.</t>
   </si>
   <si>
-    <t>2023-10-25T15:19:11Z</t>
-  </si>
-  <si>
-    <t>ac5d8492f452ea78</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.e7e2e56c3f62cf38c2bd28e614a4f738f7dc983cb92529afcbe59e2cf3c6f118.a17daefa7e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Le sezioni Piani di cura e Visite/Ricoveri e Gravidanza e Parto, esenzioni e Reti di patologia (opzionali) e Stile di vita (raccomandato) sono state omesse.
 In particolare Stile di vita e Gravidanza e Parto, gestendo la cartella clinica solo bambini in età pediatrica, non prevede la compilazione dei campi contenuti in questa sezione.</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.7afcef4901dee8ce7fd0c47083adb172245c611e427570d87803b55fd1986171.54b9e7610a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.3f0e3a3ff86bd709a0256cdfeb6a1ede099d9bf4c5640f79eab55fe2ff3b3985.eed349a820^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.56f408fd40ee70b34e5ccd255e9ea565b6c6160cfc8d8562f40b7b61778a641d.733f9503cb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.8132da4a1f045349ece4557e2eb956047029d2890a30c80dd99ceac439691927.7a7df9a171^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.76c2a5e99a8317f58512d67bebd1afa360e6d965db873450e0092fd1c0c5c514.dde38dbc11^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.7d1e3275aba5b84976147745ed257427f4c3b573d7c97748c5fd062d99e145b5.cba4353958^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-11-09T12:42:56Z</t>
+  </si>
+  <si>
+    <t>9312d7bb07f62b62</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>2023-11-09T12:45:35Z</t>
+  </si>
+  <si>
+    <t>2b36e69831168958</t>
+  </si>
+  <si>
+    <t>2023-11-09T12:57:30Z</t>
+  </si>
+  <si>
+    <t>a23263ceaa6dc1c8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.f27fc541396b207b038592265740b8c190cfb046f390cb87934af2997dc3d74c.bd56c492b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T13:00:29Z</t>
+  </si>
+  <si>
+    <t>67294e98c42b4f7a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.530b1783c3a3352aa2ee24fcf29db394df248bc15aebc9ad71dc378fd2fbc194.85b0bed068^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T13:03:23Z</t>
+  </si>
+  <si>
+    <t>b04c1738e3ed33e8</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.54eabd3c1f763af2b7d863aaa3fa8c6a3c39612fd576dbaeea276096b6be7619.cb93a8e6aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T13:05:10Z</t>
+  </si>
+  <si>
+    <t>70779f2cbbca5fb9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.3c86b2d087e4a0e2d4778865403944b629c1d6e970d2ecd37d86e55055428139.e86d87150f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T13:06:00Z</t>
+  </si>
+  <si>
+    <t>ebd568aa9da6839f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.49f76c1a99fd3081b9f6d7557110b6e38ff3bc4cb04f31a47fa43748b79d4ec5.f31f89e7f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T11:58:18Z</t>
+  </si>
+  <si>
+    <t>edcf9f249f658b4b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.147961d59df4a2b8ce08dffb6e2377e4fbe81df7cc01794a051aaa879ce3f936.9985f8afa6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T12:01:01Z</t>
+  </si>
+  <si>
+    <t>259d37d522348629</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.442cad0d64820a099ee7d33aad276c1f1bd4920047942c752dded4917b27f7d3.c2c25144bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T12:03:06Z</t>
+  </si>
+  <si>
+    <t>de7cbec633b21583</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.d473d7daff35c784e44dc4154508223bedceb942091e4de39e4343091936df1e.a57bc2b312^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T12:10:54Z</t>
+  </si>
+  <si>
+    <t>cba6572e10097a3f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.ca06870e6f2e9ce33e1667272460872a39332b8c63af7e92206ff01b40f2ff14.89591a83e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T12:14:36Z</t>
+  </si>
+  <si>
+    <t>762452563607d57d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.ee1b9bf2f173c0519dd084bb11766ba1fb767a50c93fd27352515ff926619236.c6f58eb5d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-09T12:16:43Z</t>
+  </si>
+  <si>
+    <t>6f40a8cfd56791bb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.9ea74f80d852a89564e8615f2ad42b58b86d9d330aff88819e8e9cfbb8d60ec9.e396545287^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7989,10 +7992,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G177" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I188" sqref="I188"/>
+      <selection pane="bottomRight" activeCell="I186" sqref="I186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8036,7 +8039,7 @@
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>873</v>
+        <v>857</v>
       </c>
       <c r="D2" s="40"/>
       <c r="F2" s="12"/>
@@ -9181,15 +9184,17 @@
         <v>103</v>
       </c>
       <c r="F37" s="23">
-        <v>45222</v>
+        <v>45239</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>851</v>
+        <v>870</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>852</v>
-      </c>
-      <c r="I37" s="24"/>
+        <v>871</v>
+      </c>
+      <c r="I37" s="24" t="s">
+        <v>872</v>
+      </c>
       <c r="J37" s="25" t="s">
         <v>138</v>
       </c>
@@ -9201,13 +9206,13 @@
         <v>138</v>
       </c>
       <c r="N37" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O37" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -9471,15 +9476,17 @@
         <v>125</v>
       </c>
       <c r="F45" s="23">
-        <v>45222</v>
+        <v>45239</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>855</v>
+        <v>873</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>856</v>
-      </c>
-      <c r="I45" s="24"/>
+        <v>874</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>872</v>
+      </c>
       <c r="J45" s="25" t="s">
         <v>138</v>
       </c>
@@ -9491,13 +9498,13 @@
         <v>138</v>
       </c>
       <c r="N45" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
@@ -9779,13 +9786,13 @@
         <v>138</v>
       </c>
       <c r="N53" s="25" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="O53" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P53" s="25" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">
@@ -14005,16 +14012,16 @@
         <v>383</v>
       </c>
       <c r="F177" s="23">
-        <v>45224</v>
+        <v>45239</v>
       </c>
       <c r="G177" s="24" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -14049,16 +14056,16 @@
         <v>385</v>
       </c>
       <c r="F178" s="23">
-        <v>45224</v>
+        <v>45239</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -14072,7 +14079,7 @@
       <c r="Q178" s="25"/>
       <c r="R178" s="26"/>
       <c r="S178" s="27" t="s">
-        <v>892</v>
+        <v>867</v>
       </c>
       <c r="T178" s="28" t="s">
         <v>48</v>
@@ -14095,16 +14102,16 @@
         <v>387</v>
       </c>
       <c r="F179" s="23">
-        <v>45224</v>
+        <v>45239</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>893</v>
+        <v>884</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>894</v>
+        <v>885</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>895</v>
+        <v>886</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -14118,7 +14125,7 @@
       <c r="Q179" s="25"/>
       <c r="R179" s="26"/>
       <c r="S179" s="27" t="s">
-        <v>896</v>
+        <v>868</v>
       </c>
       <c r="T179" s="28" t="s">
         <v>48</v>
@@ -14141,16 +14148,16 @@
         <v>389</v>
       </c>
       <c r="F180" s="23">
-        <v>45224</v>
+        <v>45239</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>898</v>
+        <v>888</v>
       </c>
       <c r="I180" s="24" t="s">
-        <v>899</v>
+        <v>889</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -14164,7 +14171,7 @@
       <c r="Q180" s="25"/>
       <c r="R180" s="26"/>
       <c r="S180" s="27" t="s">
-        <v>900</v>
+        <v>869</v>
       </c>
       <c r="T180" s="28" t="s">
         <v>48</v>
@@ -14187,16 +14194,16 @@
         <v>391</v>
       </c>
       <c r="F181" s="23">
-        <v>45223</v>
+        <v>45239</v>
       </c>
       <c r="G181" s="24" t="s">
-        <v>859</v>
+        <v>890</v>
       </c>
       <c r="H181" s="24" t="s">
-        <v>860</v>
+        <v>891</v>
       </c>
       <c r="I181" s="24" t="s">
-        <v>901</v>
+        <v>892</v>
       </c>
       <c r="J181" s="25" t="s">
         <v>138</v>
@@ -14209,13 +14216,13 @@
         <v>138</v>
       </c>
       <c r="N181" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O181" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P181" s="25" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="Q181" s="25"/>
       <c r="R181" s="26"/>
@@ -14241,16 +14248,16 @@
         <v>393</v>
       </c>
       <c r="F182" s="23">
-        <v>45223</v>
+        <v>45239</v>
       </c>
       <c r="G182" s="24" t="s">
-        <v>861</v>
+        <v>893</v>
       </c>
       <c r="H182" s="24" t="s">
-        <v>862</v>
+        <v>894</v>
       </c>
       <c r="I182" s="24" t="s">
-        <v>902</v>
+        <v>895</v>
       </c>
       <c r="J182" s="25" t="s">
         <v>138</v>
@@ -14263,13 +14270,13 @@
         <v>138</v>
       </c>
       <c r="N182" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O182" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P182" s="25" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="Q182" s="25"/>
       <c r="R182" s="26"/>
@@ -14295,16 +14302,16 @@
         <v>395</v>
       </c>
       <c r="F183" s="23">
-        <v>45223</v>
+        <v>45239</v>
       </c>
       <c r="G183" s="24" t="s">
-        <v>864</v>
+        <v>896</v>
       </c>
       <c r="H183" s="24" t="s">
-        <v>863</v>
+        <v>897</v>
       </c>
       <c r="I183" s="24" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="J183" s="25" t="s">
         <v>138</v>
@@ -14317,13 +14324,13 @@
         <v>138</v>
       </c>
       <c r="N183" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O183" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P183" s="25" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="Q183" s="25"/>
       <c r="R183" s="26"/>
@@ -14349,16 +14356,16 @@
         <v>397</v>
       </c>
       <c r="F184" s="23">
-        <v>45223</v>
+        <v>45239</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>866</v>
+        <v>899</v>
       </c>
       <c r="H184" s="24" t="s">
-        <v>865</v>
+        <v>900</v>
       </c>
       <c r="I184" s="24" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="J184" s="25" t="s">
         <v>138</v>
@@ -14371,13 +14378,13 @@
         <v>138</v>
       </c>
       <c r="N184" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O184" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P184" s="25" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="Q184" s="25"/>
       <c r="R184" s="26"/>
@@ -14403,16 +14410,16 @@
         <v>399</v>
       </c>
       <c r="F185" s="23">
-        <v>45223</v>
+        <v>45239</v>
       </c>
       <c r="G185" s="24" t="s">
-        <v>868</v>
+        <v>902</v>
       </c>
       <c r="H185" s="24" t="s">
-        <v>867</v>
+        <v>903</v>
       </c>
       <c r="I185" s="24" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="J185" s="25" t="s">
         <v>138</v>
@@ -14425,13 +14432,13 @@
         <v>138</v>
       </c>
       <c r="N185" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O185" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P185" s="25" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="Q185" s="25"/>
       <c r="R185" s="26"/>
@@ -14457,16 +14464,16 @@
         <v>401</v>
       </c>
       <c r="F186" s="23">
-        <v>45223</v>
+        <v>45239</v>
       </c>
       <c r="G186" s="24" t="s">
-        <v>869</v>
+        <v>905</v>
       </c>
       <c r="H186" s="24" t="s">
-        <v>870</v>
+        <v>906</v>
       </c>
       <c r="I186" s="24" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="J186" s="25" t="s">
         <v>138</v>
@@ -14479,13 +14486,13 @@
         <v>138</v>
       </c>
       <c r="N186" s="35" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O186" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P186" s="25" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="Q186" s="25"/>
       <c r="R186" s="26"/>
@@ -14518,7 +14525,7 @@
         <v>847</v>
       </c>
       <c r="K187" s="25" t="s">
-        <v>871</v>
+        <v>855</v>
       </c>
       <c r="L187" s="25"/>
       <c r="M187" s="25"/>
@@ -14556,7 +14563,7 @@
         <v>847</v>
       </c>
       <c r="K188" s="25" t="s">
-        <v>872</v>
+        <v>856</v>
       </c>
       <c r="L188" s="25"/>
       <c r="M188" s="25"/>
@@ -14594,7 +14601,7 @@
         <v>847</v>
       </c>
       <c r="K189" s="25" t="s">
-        <v>882</v>
+        <v>866</v>
       </c>
       <c r="L189" s="25"/>
       <c r="M189" s="25"/>
@@ -14632,7 +14639,7 @@
         <v>847</v>
       </c>
       <c r="K190" s="25" t="s">
-        <v>874</v>
+        <v>858</v>
       </c>
       <c r="L190" s="25"/>
       <c r="M190" s="25"/>
@@ -14670,7 +14677,7 @@
         <v>847</v>
       </c>
       <c r="K191" s="25" t="s">
-        <v>875</v>
+        <v>859</v>
       </c>
       <c r="L191" s="25"/>
       <c r="M191" s="25"/>
@@ -14708,7 +14715,7 @@
         <v>847</v>
       </c>
       <c r="K192" s="25" t="s">
-        <v>876</v>
+        <v>860</v>
       </c>
       <c r="L192" s="25"/>
       <c r="M192" s="25"/>
@@ -14746,7 +14753,7 @@
         <v>847</v>
       </c>
       <c r="K193" s="25" t="s">
-        <v>877</v>
+        <v>861</v>
       </c>
       <c r="L193" s="25"/>
       <c r="M193" s="25"/>
@@ -14784,7 +14791,7 @@
         <v>847</v>
       </c>
       <c r="K194" s="25" t="s">
-        <v>878</v>
+        <v>862</v>
       </c>
       <c r="L194" s="25"/>
       <c r="M194" s="25"/>
@@ -14822,7 +14829,7 @@
         <v>847</v>
       </c>
       <c r="K195" s="25" t="s">
-        <v>879</v>
+        <v>863</v>
       </c>
       <c r="L195" s="25"/>
       <c r="M195" s="25"/>
@@ -14860,7 +14867,7 @@
         <v>847</v>
       </c>
       <c r="K196" s="25" t="s">
-        <v>880</v>
+        <v>864</v>
       </c>
       <c r="L196" s="25"/>
       <c r="M196" s="25"/>
@@ -14898,7 +14905,7 @@
         <v>847</v>
       </c>
       <c r="K197" s="25" t="s">
-        <v>881</v>
+        <v>865</v>
       </c>
       <c r="L197" s="25"/>
       <c r="M197" s="25"/>
@@ -21185,16 +21192,16 @@
         <v>791</v>
       </c>
       <c r="F382" s="23">
-        <v>45224</v>
+        <v>45239</v>
       </c>
       <c r="G382" s="24" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="H382" s="24" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="I382" s="24" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="J382" s="25" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
aggiornamento case test Validazione PSS 170,171,172,173
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC83D705-0093-43A8-B712-22428ED0D7B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C82C36-1574-41FB-9B98-D8A7F6B0A602}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4634,42 +4634,6 @@
     <t>2.16.840.1.113883.2.9.2.200.4.4.f27fc541396b207b038592265740b8c190cfb046f390cb87934af2997dc3d74c.bd56c492b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-11-09T13:00:29Z</t>
-  </si>
-  <si>
-    <t>67294e98c42b4f7a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.530b1783c3a3352aa2ee24fcf29db394df248bc15aebc9ad71dc378fd2fbc194.85b0bed068^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-11-09T13:03:23Z</t>
-  </si>
-  <si>
-    <t>b04c1738e3ed33e8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.54eabd3c1f763af2b7d863aaa3fa8c6a3c39612fd576dbaeea276096b6be7619.cb93a8e6aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-11-09T13:05:10Z</t>
-  </si>
-  <si>
-    <t>70779f2cbbca5fb9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.3c86b2d087e4a0e2d4778865403944b629c1d6e970d2ecd37d86e55055428139.e86d87150f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-11-09T13:06:00Z</t>
-  </si>
-  <si>
-    <t>ebd568aa9da6839f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.49f76c1a99fd3081b9f6d7557110b6e38ff3bc4cb04f31a47fa43748b79d4ec5.f31f89e7f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-11-09T11:58:18Z</t>
   </si>
   <si>
@@ -4722,6 +4686,42 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.200.4.4.9ea74f80d852a89564e8615f2ad42b58b86d9d330aff88819e8e9cfbb8d60ec9.e396545287^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-29T12:00:36Z</t>
+  </si>
+  <si>
+    <t>da4cf3494d4d33e6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.2b3f39fe4e6bf627c136cf6d652a707e5d78c86a83f12ebb2a5456c2d896515f.5bc1530128^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-29T12:01:49Z</t>
+  </si>
+  <si>
+    <t>ecacc49a19fc0213</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.6235094b64c49256235080423efc270a4f5e32a0eb93ae42880834a266211bc7.4d54ad6c69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-29T12:46:28Z</t>
+  </si>
+  <si>
+    <t>d8238525cdd255ff</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.179df5adccf944056e9f373950288dab239a4b9752ed5ef14a7f9f2cabe1d486.a056f15408^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-11-29T12:05:23Z</t>
+  </si>
+  <si>
+    <t>182a5ccbcd547429</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.c6ceec063f07a53be2a19e88b60b53b12b0b9044df56ed740ff70a6cbb5b78dc.51019cd9ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7992,10 +7992,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I186" sqref="I186"/>
+      <selection pane="bottomRight" activeCell="I180" sqref="I180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14012,16 +14012,16 @@
         <v>383</v>
       </c>
       <c r="F177" s="23">
-        <v>45239</v>
+        <v>45259</v>
       </c>
       <c r="G177" s="24" t="s">
-        <v>878</v>
+        <v>896</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>879</v>
+        <v>897</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>880</v>
+        <v>898</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -14056,16 +14056,16 @@
         <v>385</v>
       </c>
       <c r="F178" s="23">
-        <v>45239</v>
+        <v>45259</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>881</v>
+        <v>899</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>882</v>
+        <v>900</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>883</v>
+        <v>901</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -14102,16 +14102,16 @@
         <v>387</v>
       </c>
       <c r="F179" s="23">
-        <v>45239</v>
+        <v>45259</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>884</v>
+        <v>902</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>885</v>
+        <v>903</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>886</v>
+        <v>904</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -14148,16 +14148,16 @@
         <v>389</v>
       </c>
       <c r="F180" s="23">
-        <v>45239</v>
+        <v>45259</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>887</v>
+        <v>905</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>888</v>
+        <v>906</v>
       </c>
       <c r="I180" s="24" t="s">
-        <v>889</v>
+        <v>907</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -14197,13 +14197,13 @@
         <v>45239</v>
       </c>
       <c r="G181" s="24" t="s">
-        <v>890</v>
+        <v>878</v>
       </c>
       <c r="H181" s="24" t="s">
-        <v>891</v>
+        <v>879</v>
       </c>
       <c r="I181" s="24" t="s">
-        <v>892</v>
+        <v>880</v>
       </c>
       <c r="J181" s="25" t="s">
         <v>138</v>
@@ -14251,13 +14251,13 @@
         <v>45239</v>
       </c>
       <c r="G182" s="24" t="s">
-        <v>893</v>
+        <v>881</v>
       </c>
       <c r="H182" s="24" t="s">
-        <v>894</v>
+        <v>882</v>
       </c>
       <c r="I182" s="24" t="s">
-        <v>895</v>
+        <v>883</v>
       </c>
       <c r="J182" s="25" t="s">
         <v>138</v>
@@ -14305,13 +14305,13 @@
         <v>45239</v>
       </c>
       <c r="G183" s="24" t="s">
-        <v>896</v>
+        <v>884</v>
       </c>
       <c r="H183" s="24" t="s">
-        <v>897</v>
+        <v>885</v>
       </c>
       <c r="I183" s="24" t="s">
-        <v>898</v>
+        <v>886</v>
       </c>
       <c r="J183" s="25" t="s">
         <v>138</v>
@@ -14359,13 +14359,13 @@
         <v>45239</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>899</v>
+        <v>887</v>
       </c>
       <c r="H184" s="24" t="s">
-        <v>900</v>
+        <v>888</v>
       </c>
       <c r="I184" s="24" t="s">
-        <v>901</v>
+        <v>889</v>
       </c>
       <c r="J184" s="25" t="s">
         <v>138</v>
@@ -14413,13 +14413,13 @@
         <v>45239</v>
       </c>
       <c r="G185" s="24" t="s">
-        <v>902</v>
+        <v>890</v>
       </c>
       <c r="H185" s="24" t="s">
-        <v>903</v>
+        <v>891</v>
       </c>
       <c r="I185" s="24" t="s">
-        <v>904</v>
+        <v>892</v>
       </c>
       <c r="J185" s="25" t="s">
         <v>138</v>
@@ -14467,13 +14467,13 @@
         <v>45239</v>
       </c>
       <c r="G186" s="24" t="s">
-        <v>905</v>
+        <v>893</v>
       </c>
       <c r="H186" s="24" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
       <c r="I186" s="24" t="s">
-        <v>907</v>
+        <v>895</v>
       </c>
       <c r="J186" s="25" t="s">
         <v>138</v>

</xml_diff>

<commit_message>
aggiornamento report-checklist.xlsx come richiesto da DTD
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C82C36-1574-41FB-9B98-D8A7F6B0A602}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F26ABD5-A208-480A-A1A0-453B7168D6E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="911">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4546,13 +4546,7 @@
     <t>Messaggio errore</t>
   </si>
   <si>
-    <t>Il PLS viene avvisato con l'errore mostrato a video e viene annullato l'invio del PS.</t>
-  </si>
-  <si>
     <t>Viene mostrato un errore a video contenente il messaggio "Impossibile contattare il servizio di validazione"</t>
-  </si>
-  <si>
-    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.</t>
   </si>
   <si>
     <t>Essendo un elemento opzionale non viene costruito l'elemento XML.</t>
@@ -4598,18 +4592,6 @@
     <t>Essendo comunque una sezione obbligatoria, non c'è modo che il medico possa omettere questa sezione nel compilare il CDA</t>
   </si>
   <si>
-    <t>Le sezioni Piani di cura e Visite/Ricoveri (opzionali) e Stile di vita (raccomandato) sono state omesse.
-In particolare Stile di vita, gestendo la cartella clinica solo bambini in età pediatrica, non prevede la compilazione dei campi contenuti in questa sezione.</t>
-  </si>
-  <si>
-    <t>Le sezioni Piani di cura e Visite/Ricoveri e Gravidanza e Parto (opzionali) e Stile di vita (raccomandato) sono state omesse.
-In particolare Stile di vita e Gravidanza e Parto, gestendo la cartella clinica solo bambini in età pediatrica, non prevede la compilazione dei campi contenuti in questa sezione.</t>
-  </si>
-  <si>
-    <t>Le sezioni Piani di cura e Visite/Ricoveri e Gravidanza e Parto, esenzioni e Reti di patologia (opzionali) e Stile di vita (raccomandato) sono state omesse.
-In particolare Stile di vita e Gravidanza e Parto, gestendo la cartella clinica solo bambini in età pediatrica, non prevede la compilazione dei campi contenuti in questa sezione.</t>
-  </si>
-  <si>
     <t>2023-11-09T12:42:56Z</t>
   </si>
   <si>
@@ -4722,6 +4704,53 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.200.4.4.c6ceec063f07a53be2a19e88b60b53b12b0b9044df56ed740ff70a6cbb5b78dc.51019cd9ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il PLS viene avvisato con l'errore mostrato a video e viene annullato l'invio del PS.
+Il test è stato effettuato per completezza e per mostrarvi l'eventuale finestra di dialogo che viene mostrata al medico in caso di errore.
+Per quanto riguarda questo specifico test non c'è possibilità da parte del medico di modificare il contenuto dei campi presenti nel token che vengono demandati completamente all'applicativo nella sua compilazione.
+In conclusione, è l'applicativo che, a priori, compila i valori del JWT e il PLS non ha nessun tipo di accesso alla sua compilazione</t>
+  </si>
+  <si>
+    <t>Il PLS viene avvisato con l'errore mostrato a video e viene annullato l'invio del PS.
+Il test è stato effettuato per completezza e per mostrarvi l'eventuale finestra di dialogo che viene mostrata al medico in caso di errore.
+Per quanto riguarda questo specifico test non c'è possibilità da parte del medico di modificare il contenuto dei campi presenti nel token che vengono demandati completamente all'applicativo nella sua compilazione.
+In conclusione, è l'applicativo che, a priori, compila i valori del JWT e il PLS non ha nessun tipo di accesso alla sua compilazione.</t>
+  </si>
+  <si>
+    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
+In questo caso, successivamente all'avviso a video al PLS, il retry è demandato completamente al medico.
+Non è implementata una coda di retry.</t>
+  </si>
+  <si>
+    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
+Il PLS non ha la possibilità di inserire un valore vuoto per quanto riguarda il confidentialityCode. 
+Il test è stato effettuato per mostrare a video eventuali errori e come vengono segnalati al medico.</t>
+  </si>
+  <si>
+    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
+Il CDA e il token JWT sono generati dinamicamente all'interno della stessa scheda del paziente per cui il PLS ha deciso di redigere il PSS e sottoporlo al processo di validazione.
+Di conseguenza utilizzando in input la stessa fonte non c'è possibilità da parte del PLS (e del conseguente invio verso i servizi di validazione) che vengano inseriti due CF differenti.
+Il test è stato effettuato per mostrare a video eventuali errori e come vengono segnalati al medico.</t>
+  </si>
+  <si>
+    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
+Qui va distinto l'errore in due casistiche : 
+a) le tag XML sono sempre presenti nel template che viene popolato dinamicamente dal PLS.
+b) mentre il loro contenuto potrebbe essere vuoto se il PLS non ha correttamente compilato l'anagrafica del paziente.
+Quindi se l'errore in esame è il caso "a", è un errore che non può mai avvenire in quanto è l'applicativo che si occupa della costruzione della struttura del template XML
+Mentre se in esame è il caso "b", allora il medico viene notificato a video dell'errore, andrà in autonomia nell'anagrafica del paziente e aggiornerà i campi come richiesto. Alla successiva richiesta di validazione che il PLS effettuerà, avendo aggiornato i valori dell'anagrafica, questi campi saranno questa volta compilati correttamente.</t>
+  </si>
+  <si>
+    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
+I valori cognome e nome sono campi obbligatori nell'inserimento del paziente all'interno dell'applicativo.
+Le tag XML sono sempre presenti in quanto demandato completamente all'applicativo, di conseguenza non possono in nessun caso essere assenti.
+In questo specifico caso inoltre anche i valori delle tag non possono essere vuoti in quanto valori fondamentali nella creazione della scheda del paziente all'interno dell'applicativo.</t>
+  </si>
+  <si>
+    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
+All'interno dell'applicativo solo M/F come sesso del paziente. E' inoltre un dato obbligatorio nella creazione della scheda del paziente.
+Può quindi assumere i valori M o F e non può mai essere vuoto.</t>
   </si>
 </sst>
 </file>
@@ -7992,10 +8021,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I180" sqref="I180"/>
+      <selection pane="bottomRight" activeCell="K193" sqref="K193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8039,7 +8068,7 @@
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D2" s="40"/>
       <c r="F2" s="12"/>
@@ -9187,13 +9216,13 @@
         <v>45239</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>138</v>
@@ -9212,7 +9241,7 @@
         <v>847</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>852</v>
+        <v>904</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -9479,13 +9508,13 @@
         <v>45239</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>138</v>
@@ -9504,7 +9533,7 @@
         <v>847</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>852</v>
+        <v>903</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
@@ -9786,13 +9815,13 @@
         <v>138</v>
       </c>
       <c r="N53" s="25" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="O53" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P53" s="25" t="s">
-        <v>854</v>
+        <v>905</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">
@@ -14015,13 +14044,13 @@
         <v>45259</v>
       </c>
       <c r="G177" s="24" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -14059,13 +14088,13 @@
         <v>45259</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>899</v>
+        <v>894</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -14078,9 +14107,7 @@
       <c r="P178" s="25"/>
       <c r="Q178" s="25"/>
       <c r="R178" s="26"/>
-      <c r="S178" s="27" t="s">
-        <v>867</v>
-      </c>
+      <c r="S178" s="27"/>
       <c r="T178" s="28" t="s">
         <v>48</v>
       </c>
@@ -14105,13 +14132,13 @@
         <v>45259</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>902</v>
+        <v>897</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>903</v>
+        <v>898</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -14124,9 +14151,7 @@
       <c r="P179" s="25"/>
       <c r="Q179" s="25"/>
       <c r="R179" s="26"/>
-      <c r="S179" s="27" t="s">
-        <v>868</v>
-      </c>
+      <c r="S179" s="27"/>
       <c r="T179" s="28" t="s">
         <v>48</v>
       </c>
@@ -14151,13 +14176,13 @@
         <v>45259</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="I180" s="24" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -14170,9 +14195,7 @@
       <c r="P180" s="25"/>
       <c r="Q180" s="25"/>
       <c r="R180" s="26"/>
-      <c r="S180" s="27" t="s">
-        <v>869</v>
-      </c>
+      <c r="S180" s="27"/>
       <c r="T180" s="28" t="s">
         <v>48</v>
       </c>
@@ -14197,13 +14220,13 @@
         <v>45239</v>
       </c>
       <c r="G181" s="24" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
       <c r="H181" s="24" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="I181" s="24" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
       <c r="J181" s="25" t="s">
         <v>138</v>
@@ -14222,7 +14245,7 @@
         <v>847</v>
       </c>
       <c r="P181" s="25" t="s">
-        <v>854</v>
+        <v>906</v>
       </c>
       <c r="Q181" s="25"/>
       <c r="R181" s="26"/>
@@ -14251,13 +14274,13 @@
         <v>45239</v>
       </c>
       <c r="G182" s="24" t="s">
-        <v>881</v>
+        <v>876</v>
       </c>
       <c r="H182" s="24" t="s">
-        <v>882</v>
+        <v>877</v>
       </c>
       <c r="I182" s="24" t="s">
-        <v>883</v>
+        <v>878</v>
       </c>
       <c r="J182" s="25" t="s">
         <v>138</v>
@@ -14276,7 +14299,7 @@
         <v>847</v>
       </c>
       <c r="P182" s="25" t="s">
-        <v>854</v>
+        <v>907</v>
       </c>
       <c r="Q182" s="25"/>
       <c r="R182" s="26"/>
@@ -14305,13 +14328,13 @@
         <v>45239</v>
       </c>
       <c r="G183" s="24" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
       <c r="H183" s="24" t="s">
-        <v>885</v>
+        <v>880</v>
       </c>
       <c r="I183" s="24" t="s">
-        <v>886</v>
+        <v>881</v>
       </c>
       <c r="J183" s="25" t="s">
         <v>138</v>
@@ -14330,7 +14353,7 @@
         <v>847</v>
       </c>
       <c r="P183" s="25" t="s">
-        <v>854</v>
+        <v>906</v>
       </c>
       <c r="Q183" s="25"/>
       <c r="R183" s="26"/>
@@ -14359,13 +14382,13 @@
         <v>45239</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="H184" s="24" t="s">
-        <v>888</v>
+        <v>883</v>
       </c>
       <c r="I184" s="24" t="s">
-        <v>889</v>
+        <v>884</v>
       </c>
       <c r="J184" s="25" t="s">
         <v>138</v>
@@ -14384,7 +14407,7 @@
         <v>847</v>
       </c>
       <c r="P184" s="25" t="s">
-        <v>854</v>
+        <v>908</v>
       </c>
       <c r="Q184" s="25"/>
       <c r="R184" s="26"/>
@@ -14413,13 +14436,13 @@
         <v>45239</v>
       </c>
       <c r="G185" s="24" t="s">
-        <v>890</v>
+        <v>885</v>
       </c>
       <c r="H185" s="24" t="s">
-        <v>891</v>
+        <v>886</v>
       </c>
       <c r="I185" s="24" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
       <c r="J185" s="25" t="s">
         <v>138</v>
@@ -14438,7 +14461,7 @@
         <v>847</v>
       </c>
       <c r="P185" s="25" t="s">
-        <v>854</v>
+        <v>909</v>
       </c>
       <c r="Q185" s="25"/>
       <c r="R185" s="26"/>
@@ -14467,13 +14490,13 @@
         <v>45239</v>
       </c>
       <c r="G186" s="24" t="s">
-        <v>893</v>
+        <v>888</v>
       </c>
       <c r="H186" s="24" t="s">
-        <v>894</v>
+        <v>889</v>
       </c>
       <c r="I186" s="24" t="s">
-        <v>895</v>
+        <v>890</v>
       </c>
       <c r="J186" s="25" t="s">
         <v>138</v>
@@ -14492,7 +14515,7 @@
         <v>847</v>
       </c>
       <c r="P186" s="25" t="s">
-        <v>854</v>
+        <v>910</v>
       </c>
       <c r="Q186" s="25"/>
       <c r="R186" s="26"/>
@@ -14525,7 +14548,7 @@
         <v>847</v>
       </c>
       <c r="K187" s="25" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="L187" s="25"/>
       <c r="M187" s="25"/>
@@ -14563,7 +14586,7 @@
         <v>847</v>
       </c>
       <c r="K188" s="25" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="L188" s="25"/>
       <c r="M188" s="25"/>
@@ -14601,7 +14624,7 @@
         <v>847</v>
       </c>
       <c r="K189" s="25" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="L189" s="25"/>
       <c r="M189" s="25"/>
@@ -14639,7 +14662,7 @@
         <v>847</v>
       </c>
       <c r="K190" s="25" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="L190" s="25"/>
       <c r="M190" s="25"/>
@@ -14677,7 +14700,7 @@
         <v>847</v>
       </c>
       <c r="K191" s="25" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="L191" s="25"/>
       <c r="M191" s="25"/>
@@ -14715,7 +14738,7 @@
         <v>847</v>
       </c>
       <c r="K192" s="25" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="L192" s="25"/>
       <c r="M192" s="25"/>
@@ -14753,7 +14776,7 @@
         <v>847</v>
       </c>
       <c r="K193" s="25" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="L193" s="25"/>
       <c r="M193" s="25"/>
@@ -14791,7 +14814,7 @@
         <v>847</v>
       </c>
       <c r="K194" s="25" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="L194" s="25"/>
       <c r="M194" s="25"/>
@@ -14829,7 +14852,7 @@
         <v>847</v>
       </c>
       <c r="K195" s="25" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="L195" s="25"/>
       <c r="M195" s="25"/>
@@ -14867,7 +14890,7 @@
         <v>847</v>
       </c>
       <c r="K196" s="25" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="L196" s="25"/>
       <c r="M196" s="25"/>
@@ -14905,7 +14928,7 @@
         <v>847</v>
       </c>
       <c r="K197" s="25" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="L197" s="25"/>
       <c r="M197" s="25"/>
@@ -21195,13 +21218,13 @@
         <v>45239</v>
       </c>
       <c r="G382" s="24" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="H382" s="24" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="I382" s="24" t="s">
-        <v>877</v>
+        <v>872</v>
       </c>
       <c r="J382" s="25" t="s">
         <v>138</v>
@@ -27633,8 +27656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18989C3-D939-4409-BAFF-AA4268B3BADE}">
   <dimension ref="A1:A110"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
aggiornamento casi di test 176 e 179
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F26ABD5-A208-480A-A1A0-453B7168D6E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F91BD4-8A3E-4208-B81C-2738C5C37F09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="906">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4634,15 +4634,6 @@
     <t>2.16.840.1.113883.2.9.2.200.4.4.442cad0d64820a099ee7d33aad276c1f1bd4920047942c752dded4917b27f7d3.c2c25144bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-11-09T12:03:06Z</t>
-  </si>
-  <si>
-    <t>de7cbec633b21583</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.d473d7daff35c784e44dc4154508223bedceb942091e4de39e4343091936df1e.a57bc2b312^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-11-09T12:10:54Z</t>
   </si>
   <si>
@@ -4659,15 +4650,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.200.4.4.ee1b9bf2f173c0519dd084bb11766ba1fb767a50c93fd27352515ff926619236.c6f58eb5d4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-11-09T12:16:43Z</t>
-  </si>
-  <si>
-    <t>6f40a8cfd56791bb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.9ea74f80d852a89564e8615f2ad42b58b86d9d330aff88819e8e9cfbb8d60ec9.e396545287^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2023-11-29T12:00:36Z</t>
@@ -4748,9 +4730,13 @@
 In questo specifico caso inoltre anche i valori delle tag non possono essere vuoti in quanto valori fondamentali nella creazione della scheda del paziente all'interno dell'applicativo.</t>
   </si>
   <si>
-    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
-All'interno dell'applicativo solo M/F come sesso del paziente. E' inoltre un dato obbligatorio nella creazione della scheda del paziente.
-Può quindi assumere i valori M o F e non può mai essere vuoto.</t>
+    <t>Il valore del sesso del paziente all'interno del programma può assumere solo i valori M o F e nessun altro tipo di valore è associabile al paziente.
+Il medico non ha la possibilità di inserire il sesso del paziente in maniera testuale in nessun punto dell'applicativo, incluse tutte le sezioni che vengono utilizzate per popolare il PSS.
+NON esiste quindi alcuna possibilità che l'errore del caso di test si presenti.</t>
+  </si>
+  <si>
+    <t>Il medico non ha possibilità di impostare il valore "R" (Restricted) da interfaccia in quanto sono presenti solo i valori N e V.
+Non è presente alcuna forzatura da interfaccia che permetta l'inserimento del valore N da parte del PLS.</t>
   </si>
 </sst>
 </file>
@@ -5579,50 +5565,6 @@
         <a:xfrm>
           <a:off x="0" y="15621000"/>
           <a:ext cx="7430537" cy="2000529"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600925</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>143161</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Immagine 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEAC1DCF-EC87-409C-BDA8-43BDC682C24C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="18288000"/>
-          <a:ext cx="6087325" cy="2048161"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8021,10 +7963,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K193" sqref="K193"/>
+      <selection pane="bottomRight" activeCell="I192" sqref="I192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9241,7 +9183,7 @@
         <v>847</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -9533,7 +9475,7 @@
         <v>847</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
@@ -9821,7 +9763,7 @@
         <v>847</v>
       </c>
       <c r="P53" s="25" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">
@@ -14044,13 +13986,13 @@
         <v>45259</v>
       </c>
       <c r="G177" s="24" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -14088,13 +14030,13 @@
         <v>45259</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -14132,13 +14074,13 @@
         <v>45259</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -14176,13 +14118,13 @@
         <v>45259</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="I180" s="24" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -14245,7 +14187,7 @@
         <v>847</v>
       </c>
       <c r="P181" s="25" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="Q181" s="25"/>
       <c r="R181" s="26"/>
@@ -14299,7 +14241,7 @@
         <v>847</v>
       </c>
       <c r="P182" s="25" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="Q182" s="25"/>
       <c r="R182" s="26"/>
@@ -14324,37 +14266,21 @@
       <c r="E183" s="22" t="s">
         <v>395</v>
       </c>
-      <c r="F183" s="23">
-        <v>45239</v>
-      </c>
-      <c r="G183" s="24" t="s">
-        <v>879</v>
-      </c>
-      <c r="H183" s="24" t="s">
-        <v>880</v>
-      </c>
-      <c r="I183" s="24" t="s">
-        <v>881</v>
-      </c>
+      <c r="F183" s="23"/>
+      <c r="G183" s="24"/>
+      <c r="H183" s="24"/>
+      <c r="I183" s="24"/>
       <c r="J183" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="K183" s="25"/>
-      <c r="L183" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="M183" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="N183" s="35" t="s">
-        <v>851</v>
-      </c>
-      <c r="O183" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="P183" s="25" t="s">
-        <v>906</v>
-      </c>
+      <c r="K183" s="25" t="s">
+        <v>905</v>
+      </c>
+      <c r="L183" s="25"/>
+      <c r="M183" s="25"/>
+      <c r="N183" s="35"/>
+      <c r="O183" s="25"/>
+      <c r="P183" s="25"/>
       <c r="Q183" s="25"/>
       <c r="R183" s="26"/>
       <c r="S183" s="27"/>
@@ -14382,13 +14308,13 @@
         <v>45239</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="H184" s="24" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="I184" s="24" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="J184" s="25" t="s">
         <v>138</v>
@@ -14407,7 +14333,7 @@
         <v>847</v>
       </c>
       <c r="P184" s="25" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="Q184" s="25"/>
       <c r="R184" s="26"/>
@@ -14436,13 +14362,13 @@
         <v>45239</v>
       </c>
       <c r="G185" s="24" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="H185" s="24" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="I185" s="24" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="J185" s="25" t="s">
         <v>138</v>
@@ -14461,7 +14387,7 @@
         <v>847</v>
       </c>
       <c r="P185" s="25" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="Q185" s="25"/>
       <c r="R185" s="26"/>
@@ -14486,37 +14412,21 @@
       <c r="E186" s="22" t="s">
         <v>401</v>
       </c>
-      <c r="F186" s="23">
-        <v>45239</v>
-      </c>
-      <c r="G186" s="24" t="s">
-        <v>888</v>
-      </c>
-      <c r="H186" s="24" t="s">
-        <v>889</v>
-      </c>
-      <c r="I186" s="24" t="s">
-        <v>890</v>
-      </c>
+      <c r="F186" s="23"/>
+      <c r="G186" s="24"/>
+      <c r="H186" s="24"/>
+      <c r="I186" s="24"/>
       <c r="J186" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="K186" s="25"/>
-      <c r="L186" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="M186" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="N186" s="35" t="s">
-        <v>851</v>
-      </c>
-      <c r="O186" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="P186" s="25" t="s">
-        <v>910</v>
-      </c>
+      <c r="K186" s="25" t="s">
+        <v>904</v>
+      </c>
+      <c r="L186" s="25"/>
+      <c r="M186" s="25"/>
+      <c r="N186" s="35"/>
+      <c r="O186" s="25"/>
+      <c r="P186" s="25"/>
       <c r="Q186" s="25"/>
       <c r="R186" s="26"/>
       <c r="S186" s="27"/>
@@ -25949,10 +25859,8 @@
     <hyperlink ref="N45" location="'Errori interfaccia'!A14" display="Messaggio errore" xr:uid="{B7024710-AD82-4305-9A00-1B9A64886F37}"/>
     <hyperlink ref="N181" location="'Errori interfaccia'!A28" display="Messaggio errore" xr:uid="{AB25E56D-44AF-4322-8392-581FE98872B2}"/>
     <hyperlink ref="N182" location="'Errori interfaccia'!A41" display="Messaggio errore" xr:uid="{F62D03FF-71B6-424D-AEF8-56D6A211B74F}"/>
-    <hyperlink ref="N183" location="'Errori interfaccia'!A54" display="Messaggio errore" xr:uid="{C2448E11-E614-4964-AC15-0BDA0675A88B}"/>
     <hyperlink ref="N184" location="'Errori interfaccia'!A68" display="Messaggio errore" xr:uid="{0F522CC9-9DD3-458B-95C4-045AEF1BF39E}"/>
     <hyperlink ref="N185" location="'Errori interfaccia'!A82" display="Messaggio errore" xr:uid="{618CB0DF-90EE-4D63-B1E9-ECF2F14DEA9B}"/>
-    <hyperlink ref="N186" location="'Errori interfaccia'!A96" display="Messaggio errore" xr:uid="{03702F02-D62E-4A59-906F-40FDDA70CB74}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -27656,8 +27564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18989C3-D939-4409-BAFF-AA4268B3BADE}">
   <dimension ref="A1:A110"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27698,11 +27606,6 @@
     <row r="82" spans="1:1">
       <c r="A82" s="34" t="s">
         <v>398</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="110" spans="1:1">

</xml_diff>

<commit_message>
aggiornamento casi test 176 e 179
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F91BD4-8A3E-4208-B81C-2738C5C37F09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F6837E-8401-4B38-9DB7-B69F1E651984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="912">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4730,13 +4730,34 @@
 In questo specifico caso inoltre anche i valori delle tag non possono essere vuoti in quanto valori fondamentali nella creazione della scheda del paziente all'interno dell'applicativo.</t>
   </si>
   <si>
-    <t>Il valore del sesso del paziente all'interno del programma può assumere solo i valori M o F e nessun altro tipo di valore è associabile al paziente.
-Il medico non ha la possibilità di inserire il sesso del paziente in maniera testuale in nessun punto dell'applicativo, incluse tutte le sezioni che vengono utilizzate per popolare il PSS.
-NON esiste quindi alcuna possibilità che l'errore del caso di test si presenti.</t>
-  </si>
-  <si>
-    <t>Il medico non ha possibilità di impostare il valore "R" (Restricted) da interfaccia in quanto sono presenti solo i valori N e V.
-Non è presente alcuna forzatura da interfaccia che permetta l'inserimento del valore N da parte del PLS.</t>
+    <t>2024-01-12T12:08:10Z</t>
+  </si>
+  <si>
+    <t>cc5062f21e7fe4d4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.37c449c9b7a13ce7593c48d13d355d2d9fb96ebf08b1cd150589a74ce3e9aed4.0cd78317c5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il caso d'uso è stato simulato per potervi permettere di visualizzare l'errore nel caso in cui venga erroneamente (da sorgente per un refuso nel codice) impostato il valore "R" (Restricted) nel CDA.
+L'errore, come precedentemente segnalato, nella logica applicativa di Junior Bit non è applicabile dato che in interfaccia il PLS NON ha la possibilità di poter volontariamente o involontariamente inserire questo valore.
+Dovendo, per il solo caso d'uso del test, mostrarvi come si comporterebbe il programma, viene mostrato a video l'errore presente nel json di risposta.
+Ci tengo a sottolineare che il caso d'uso nasce non applicabile, per i motivi di cui sopra,  per TUTTI i PLS che usano il nostro applicativo, ma non potendo tornare indietro rispetto a quanto vi avevamo riportato negli scorsi merge, il test deve essere impostato in questo modo.</t>
+  </si>
+  <si>
+    <t>2024-01-12T13:10:29Z</t>
+  </si>
+  <si>
+    <t>a097e6a8e480c223</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.a8a746538b78a2a407548b56f7bcd18f807a36663f0141425c22e69096a8016d.3bdeadb8e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il caso d'uso è stato simulato per potervi permettere di visualizzare l'errore nel caso in cui venga erroneamente (da sorgente per un refuso nel codice) impostato il valore "NB" (Not Binary) nel CDA.
+L'errore, come precedentemente segnalato, nella logica applicativa di Junior Bit non è applicabile dato che in interfaccia il PLS NON ha la possibilità di poter volontariamente o involontariamente inserire questo valore.
+Dovendo, per il solo caso d'uso del test, mostrarvi come si comporterebbe il programma, viene mostrato a video l'errore presente nel json di risposta.
+Ci tengo a sottolineare che il caso d'uso nasce non applicabile, per i motivi di cui sopra,  per TUTTI i PLS che usano il nostro applicativo, ma non potendo tornare indietro rispetto a quanto vi avevamo riportato negli scorsi merge, il test deve essere impostato in questo modo.</t>
   </si>
 </sst>
 </file>
@@ -4746,7 +4767,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4804,6 +4825,12 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -5067,7 +5094,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5184,6 +5211,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7963,10 +7993,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I192" sqref="I192"/>
+      <selection pane="bottomRight" activeCell="N189" sqref="N189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14266,21 +14296,35 @@
       <c r="E183" s="22" t="s">
         <v>395</v>
       </c>
-      <c r="F183" s="23"/>
-      <c r="G183" s="24"/>
-      <c r="H183" s="24"/>
-      <c r="I183" s="24"/>
+      <c r="F183" s="23">
+        <v>45303</v>
+      </c>
+      <c r="G183" s="24" t="s">
+        <v>904</v>
+      </c>
+      <c r="H183" s="24" t="s">
+        <v>905</v>
+      </c>
+      <c r="I183" s="24" t="s">
+        <v>906</v>
+      </c>
       <c r="J183" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K183" s="25"/>
+      <c r="L183" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="M183" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="N183" s="35"/>
+      <c r="O183" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K183" s="25" t="s">
-        <v>905</v>
-      </c>
-      <c r="L183" s="25"/>
-      <c r="M183" s="25"/>
-      <c r="N183" s="35"/>
-      <c r="O183" s="25"/>
-      <c r="P183" s="25"/>
+      <c r="P183" s="49" t="s">
+        <v>907</v>
+      </c>
       <c r="Q183" s="25"/>
       <c r="R183" s="26"/>
       <c r="S183" s="27"/>
@@ -14412,21 +14456,35 @@
       <c r="E186" s="22" t="s">
         <v>401</v>
       </c>
-      <c r="F186" s="23"/>
-      <c r="G186" s="24"/>
-      <c r="H186" s="24"/>
-      <c r="I186" s="24"/>
+      <c r="F186" s="23">
+        <v>45303</v>
+      </c>
+      <c r="G186" s="24" t="s">
+        <v>908</v>
+      </c>
+      <c r="H186" s="24" t="s">
+        <v>909</v>
+      </c>
+      <c r="I186" s="24" t="s">
+        <v>910</v>
+      </c>
       <c r="J186" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K186" s="25"/>
+      <c r="L186" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="M186" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="N186" s="35"/>
+      <c r="O186" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="K186" s="25" t="s">
-        <v>904</v>
-      </c>
-      <c r="L186" s="25"/>
-      <c r="M186" s="25"/>
-      <c r="N186" s="35"/>
-      <c r="O186" s="25"/>
-      <c r="P186" s="25"/>
+      <c r="P186" s="25" t="s">
+        <v>911</v>
+      </c>
       <c r="Q186" s="25"/>
       <c r="R186" s="26"/>
       <c r="S186" s="27"/>
@@ -25863,8 +25921,8 @@
     <hyperlink ref="N185" location="'Errori interfaccia'!A82" display="Messaggio errore" xr:uid="{618CB0DF-90EE-4D63-B1E9-ECF2F14DEA9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
aggiornamento case test 174 e 179 come richiesto
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACCREDITAMENTO GATEWAY\it-fse-accreditamento\GATEWAY\A1#111JUNIORBIT00\SOSEPE_S.R.L\JUNIORBIT\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F6837E-8401-4B38-9DB7-B69F1E651984}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB4996-B8EB-470B-9B64-A47E065EBF5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="906">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4616,15 +4616,6 @@
     <t>2.16.840.1.113883.2.9.2.200.4.4.f27fc541396b207b038592265740b8c190cfb046f390cb87934af2997dc3d74c.bd56c492b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-11-09T11:58:18Z</t>
-  </si>
-  <si>
-    <t>edcf9f249f658b4b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.147961d59df4a2b8ce08dffb6e2377e4fbe81df7cc01794a051aaa879ce3f936.9985f8afa6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-11-09T12:01:01Z</t>
   </si>
   <si>
@@ -4703,11 +4694,6 @@
     <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
 In questo caso, successivamente all'avviso a video al PLS, il retry è demandato completamente al medico.
 Non è implementata una coda di retry.</t>
-  </si>
-  <si>
-    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
-Il PLS non ha la possibilità di inserire un valore vuoto per quanto riguarda il confidentialityCode. 
-Il test è stato effettuato per mostrare a video eventuali errori e come vengono segnalati al medico.</t>
   </si>
   <si>
     <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
@@ -4745,19 +4731,12 @@
 Ci tengo a sottolineare che il caso d'uso nasce non applicabile, per i motivi di cui sopra,  per TUTTI i PLS che usano il nostro applicativo, ma non potendo tornare indietro rispetto a quanto vi avevamo riportato negli scorsi merge, il test deve essere impostato in questo modo.</t>
   </si>
   <si>
-    <t>2024-01-12T13:10:29Z</t>
-  </si>
-  <si>
-    <t>a097e6a8e480c223</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.a8a746538b78a2a407548b56f7bcd18f807a36663f0141425c22e69096a8016d.3bdeadb8e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Il caso d'uso è stato simulato per potervi permettere di visualizzare l'errore nel caso in cui venga erroneamente (da sorgente per un refuso nel codice) impostato il valore "NB" (Not Binary) nel CDA.
-L'errore, come precedentemente segnalato, nella logica applicativa di Junior Bit non è applicabile dato che in interfaccia il PLS NON ha la possibilità di poter volontariamente o involontariamente inserire questo valore.
-Dovendo, per il solo caso d'uso del test, mostrarvi come si comporterebbe il programma, viene mostrato a video l'errore presente nel json di risposta.
-Ci tengo a sottolineare che il caso d'uso nasce non applicabile, per i motivi di cui sopra,  per TUTTI i PLS che usano il nostro applicativo, ma non potendo tornare indietro rispetto a quanto vi avevamo riportato negli scorsi merge, il test deve essere impostato in questo modo.</t>
+    <t>Il valore di default dell'applicativo è "N" o "V" in base alla scelta del medico PLS.
+NON ha la possibilità di omettere questo valore durante la compilazione del CDA.</t>
+  </si>
+  <si>
+    <t>Il sesso del paziente è un campo obbligatorio durante la creazione del paziente all'interno della nostra cartella.
+Gli unici valori possibili sono "M" o "F", non c'è quindi possibilità da parte del medico PLS durante la compilazione del CDA di inserire altri valori.</t>
   </si>
 </sst>
 </file>
@@ -5190,6 +5169,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5211,9 +5193,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5387,50 +5366,6 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>87013</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Immagine 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{242D6C04-0CAD-42D6-8744-6150C2DD5A6A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="5334000"/>
-          <a:ext cx="9231013" cy="2105025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -5454,7 +5389,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5498,7 +5433,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5542,7 +5477,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5586,7 +5521,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -7993,10 +7928,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N189" sqref="N189"/>
+      <selection pane="bottomRight" activeCell="K186" sqref="K186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -8035,14 +7970,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42" t="s">
         <v>855</v>
       </c>
-      <c r="D2" s="40"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -8060,14 +7995,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>849</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -8085,12 +8020,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="48" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>848</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -8109,12 +8044,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>850</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -8132,8 +8067,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -9213,7 +9148,7 @@
         <v>847</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -9505,7 +9440,7 @@
         <v>847</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
@@ -9793,7 +9728,7 @@
         <v>847</v>
       </c>
       <c r="P53" s="25" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">
@@ -14016,13 +13951,13 @@
         <v>45259</v>
       </c>
       <c r="G177" s="24" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -14060,13 +13995,13 @@
         <v>45259</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -14104,13 +14039,13 @@
         <v>45259</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -14148,13 +14083,13 @@
         <v>45259</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="I180" s="24" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -14188,37 +14123,21 @@
       <c r="E181" s="22" t="s">
         <v>391</v>
       </c>
-      <c r="F181" s="23">
-        <v>45239</v>
-      </c>
-      <c r="G181" s="24" t="s">
-        <v>873</v>
-      </c>
-      <c r="H181" s="24" t="s">
-        <v>874</v>
-      </c>
-      <c r="I181" s="24" t="s">
-        <v>875</v>
-      </c>
+      <c r="F181" s="23"/>
+      <c r="G181" s="24"/>
+      <c r="H181" s="24"/>
+      <c r="I181" s="24"/>
       <c r="J181" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="K181" s="25"/>
-      <c r="L181" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="M181" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="N181" s="35" t="s">
-        <v>851</v>
-      </c>
-      <c r="O181" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="P181" s="25" t="s">
-        <v>900</v>
-      </c>
+      <c r="K181" s="25" t="s">
+        <v>904</v>
+      </c>
+      <c r="L181" s="25"/>
+      <c r="M181" s="25"/>
+      <c r="N181" s="35"/>
+      <c r="O181" s="25"/>
+      <c r="P181" s="25"/>
       <c r="Q181" s="25"/>
       <c r="R181" s="26"/>
       <c r="S181" s="27"/>
@@ -14246,13 +14165,13 @@
         <v>45239</v>
       </c>
       <c r="G182" s="24" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="H182" s="24" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="I182" s="24" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="J182" s="25" t="s">
         <v>138</v>
@@ -14271,7 +14190,7 @@
         <v>847</v>
       </c>
       <c r="P182" s="25" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
       <c r="Q182" s="25"/>
       <c r="R182" s="26"/>
@@ -14300,13 +14219,13 @@
         <v>45303</v>
       </c>
       <c r="G183" s="24" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
       <c r="H183" s="24" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="I183" s="24" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="J183" s="25" t="s">
         <v>138</v>
@@ -14322,8 +14241,8 @@
       <c r="O183" s="25" t="s">
         <v>847</v>
       </c>
-      <c r="P183" s="49" t="s">
-        <v>907</v>
+      <c r="P183" s="37" t="s">
+        <v>903</v>
       </c>
       <c r="Q183" s="25"/>
       <c r="R183" s="26"/>
@@ -14352,13 +14271,13 @@
         <v>45239</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="H184" s="24" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="I184" s="24" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="J184" s="25" t="s">
         <v>138</v>
@@ -14377,7 +14296,7 @@
         <v>847</v>
       </c>
       <c r="P184" s="25" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
       <c r="Q184" s="25"/>
       <c r="R184" s="26"/>
@@ -14406,13 +14325,13 @@
         <v>45239</v>
       </c>
       <c r="G185" s="24" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="H185" s="24" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="I185" s="24" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="J185" s="25" t="s">
         <v>138</v>
@@ -14431,7 +14350,7 @@
         <v>847</v>
       </c>
       <c r="P185" s="25" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
       <c r="Q185" s="25"/>
       <c r="R185" s="26"/>
@@ -14456,35 +14375,21 @@
       <c r="E186" s="22" t="s">
         <v>401</v>
       </c>
-      <c r="F186" s="23">
-        <v>45303</v>
-      </c>
-      <c r="G186" s="24" t="s">
-        <v>908</v>
-      </c>
-      <c r="H186" s="24" t="s">
-        <v>909</v>
-      </c>
-      <c r="I186" s="24" t="s">
-        <v>910</v>
-      </c>
+      <c r="F186" s="23"/>
+      <c r="G186" s="24"/>
+      <c r="H186" s="24"/>
+      <c r="I186" s="24"/>
       <c r="J186" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="K186" s="25"/>
-      <c r="L186" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="M186" s="25" t="s">
-        <v>138</v>
-      </c>
+        <v>847</v>
+      </c>
+      <c r="K186" s="25" t="s">
+        <v>905</v>
+      </c>
+      <c r="L186" s="25"/>
+      <c r="M186" s="25"/>
       <c r="N186" s="35"/>
-      <c r="O186" s="25" t="s">
-        <v>847</v>
-      </c>
-      <c r="P186" s="25" t="s">
-        <v>911</v>
-      </c>
+      <c r="O186" s="25"/>
+      <c r="P186" s="25"/>
       <c r="Q186" s="25"/>
       <c r="R186" s="26"/>
       <c r="S186" s="27"/>
@@ -25915,7 +25820,6 @@
   <hyperlinks>
     <hyperlink ref="N37" location="'Errori interfaccia'!A1" display="Messaggio errore" xr:uid="{77C411A4-8CB7-46B0-8CF4-C36DD93EEB82}"/>
     <hyperlink ref="N45" location="'Errori interfaccia'!A14" display="Messaggio errore" xr:uid="{B7024710-AD82-4305-9A00-1B9A64886F37}"/>
-    <hyperlink ref="N181" location="'Errori interfaccia'!A28" display="Messaggio errore" xr:uid="{AB25E56D-44AF-4322-8392-581FE98872B2}"/>
     <hyperlink ref="N182" location="'Errori interfaccia'!A41" display="Messaggio errore" xr:uid="{F62D03FF-71B6-424D-AEF8-56D6A211B74F}"/>
     <hyperlink ref="N184" location="'Errori interfaccia'!A68" display="Messaggio errore" xr:uid="{0F522CC9-9DD3-458B-95C4-045AEF1BF39E}"/>
     <hyperlink ref="N185" location="'Errori interfaccia'!A82" display="Messaggio errore" xr:uid="{618CB0DF-90EE-4D63-B1E9-ECF2F14DEA9B}"/>
@@ -27622,8 +27526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18989C3-D939-4409-BAFF-AA4268B3BADE}">
   <dimension ref="A1:A110"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27639,11 +27543,6 @@
     <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="41" spans="1:1">

</xml_diff>

<commit_message>
aggiornamento case test 30,38, 172 e 176 come richiesto
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACCREDITAMENTO GATEWAY\it-fse-accreditamento\GATEWAY\A1#111JUNIORBIT00\SOSEPE_S.R.L\JUNIORBIT\7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69906C34-26D7-49C7-BAA5-66BF4B3ED64A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0349C165-96E9-45EE-8106-54C40AD4A99B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4592,21 +4592,9 @@
     <t>Essendo comunque una sezione obbligatoria, non c'è modo che il medico possa omettere questa sezione nel compilare il CDA</t>
   </si>
   <si>
-    <t>2023-11-09T12:42:56Z</t>
-  </si>
-  <si>
-    <t>9312d7bb07f62b62</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2023-11-09T12:45:35Z</t>
-  </si>
-  <si>
-    <t>2b36e69831168958</t>
-  </si>
-  <si>
     <t>2023-11-09T12:57:30Z</t>
   </si>
   <si>
@@ -4659,15 +4647,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.200.4.4.6235094b64c49256235080423efc270a4f5e32a0eb93ae42880834a266211bc7.4d54ad6c69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-11-29T12:46:28Z</t>
-  </si>
-  <si>
-    <t>d8238525cdd255ff</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.179df5adccf944056e9f373950288dab239a4b9752ed5ef14a7f9f2cabe1d486.a056f15408^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2023-11-29T12:05:23Z</t>
@@ -4716,15 +4695,6 @@
 In questo specifico caso inoltre anche i valori delle tag non possono essere vuoti in quanto valori fondamentali nella creazione della scheda del paziente all'interno dell'applicativo.</t>
   </si>
   <si>
-    <t>2024-01-12T12:08:10Z</t>
-  </si>
-  <si>
-    <t>cc5062f21e7fe4d4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.37c449c9b7a13ce7593c48d13d355d2d9fb96ebf08b1cd150589a74ce3e9aed4.0cd78317c5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il caso d'uso è stato simulato per potervi permettere di visualizzare l'errore nel caso in cui venga erroneamente (da sorgente per un refuso nel codice) impostato il valore "R" (Restricted) nel CDA.
 L'errore, come precedentemente segnalato, nella logica applicativa di Junior Bit non è applicabile dato che in interfaccia il PLS NON ha la possibilità di poter volontariamente o involontariamente inserire questo valore.
 Dovendo, per il solo caso d'uso del test, mostrarvi come si comporterebbe il programma, viene mostrato a video l'errore presente nel json di risposta.
@@ -4737,6 +4707,36 @@
   <si>
     <t>Il sesso del paziente è un campo obbligatorio durante la creazione del paziente all'interno della nostra cartella.
 Gli unici valori possibili sono "M" o "F", non c'è quindi possibilità da parte del medico PLS durante la compilazione del CDA di inserire altri valori.</t>
+  </si>
+  <si>
+    <t>2024-01-29T14:17:57Z</t>
+  </si>
+  <si>
+    <t>1373d9a6af7044db</t>
+  </si>
+  <si>
+    <t>2024-01-29T14:24:14Z</t>
+  </si>
+  <si>
+    <t>fae42361425536ee</t>
+  </si>
+  <si>
+    <t>2024-01-29T14:29:34Z</t>
+  </si>
+  <si>
+    <t>855cc176cbf077dc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.c2eff106af91871f74c0c5829c458b7a92b62b65618e9190e7193cc1cab04f04.e63c6f5804^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-01-29T15:55:45Z</t>
+  </si>
+  <si>
+    <t>240336b3e6d9300b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.aac6f2c803a5069fa7b90243003ff2e987782111c5b8d9f219bd595628a842a3.267f2aed2e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7928,10 +7928,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="N183" sqref="N183"/>
+      <selection pane="bottomRight" activeCell="A183" sqref="A183:XFD183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -9120,16 +9120,16 @@
         <v>103</v>
       </c>
       <c r="F37" s="23">
-        <v>45239</v>
+        <v>45320</v>
       </c>
       <c r="G37" s="24" t="s">
+        <v>896</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>897</v>
+      </c>
+      <c r="I37" s="24" t="s">
         <v>865</v>
-      </c>
-      <c r="H37" s="24" t="s">
-        <v>866</v>
-      </c>
-      <c r="I37" s="24" t="s">
-        <v>867</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>138</v>
@@ -9148,7 +9148,7 @@
         <v>847</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -9412,16 +9412,16 @@
         <v>125</v>
       </c>
       <c r="F45" s="23">
-        <v>45239</v>
+        <v>45320</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>868</v>
+        <v>898</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>869</v>
+        <v>899</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>138</v>
@@ -9440,7 +9440,7 @@
         <v>847</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
@@ -9728,7 +9728,7 @@
         <v>847</v>
       </c>
       <c r="P53" s="25" t="s">
-        <v>896</v>
+        <v>889</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">
@@ -13951,13 +13951,13 @@
         <v>45259</v>
       </c>
       <c r="G177" s="24" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="I177" s="24" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -13995,13 +13995,13 @@
         <v>45259</v>
       </c>
       <c r="G178" s="24" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
       <c r="H178" s="24" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="I178" s="24" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -14036,16 +14036,16 @@
         <v>387</v>
       </c>
       <c r="F179" s="23">
-        <v>45259</v>
+        <v>45320</v>
       </c>
       <c r="G179" s="24" t="s">
-        <v>888</v>
+        <v>903</v>
       </c>
       <c r="H179" s="24" t="s">
-        <v>889</v>
+        <v>904</v>
       </c>
       <c r="I179" s="24" t="s">
-        <v>890</v>
+        <v>905</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -14083,13 +14083,13 @@
         <v>45259</v>
       </c>
       <c r="G180" s="24" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="H180" s="24" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="I180" s="24" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -14131,7 +14131,7 @@
         <v>847</v>
       </c>
       <c r="K181" s="25" t="s">
-        <v>904</v>
+        <v>894</v>
       </c>
       <c r="L181" s="25"/>
       <c r="M181" s="25"/>
@@ -14165,13 +14165,13 @@
         <v>45239</v>
       </c>
       <c r="G182" s="24" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="H182" s="24" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="I182" s="24" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
       <c r="J182" s="25" t="s">
         <v>138</v>
@@ -14190,7 +14190,7 @@
         <v>847</v>
       </c>
       <c r="P182" s="25" t="s">
-        <v>897</v>
+        <v>890</v>
       </c>
       <c r="Q182" s="25"/>
       <c r="R182" s="26"/>
@@ -14216,7 +14216,7 @@
         <v>395</v>
       </c>
       <c r="F183" s="23">
-        <v>45303</v>
+        <v>45320</v>
       </c>
       <c r="G183" s="24" t="s">
         <v>900</v>
@@ -14244,7 +14244,7 @@
         <v>847</v>
       </c>
       <c r="P183" s="37" t="s">
-        <v>903</v>
+        <v>893</v>
       </c>
       <c r="Q183" s="25"/>
       <c r="R183" s="26"/>
@@ -14273,13 +14273,13 @@
         <v>45239</v>
       </c>
       <c r="G184" s="24" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
       <c r="H184" s="24" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="I184" s="24" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="J184" s="25" t="s">
         <v>138</v>
@@ -14298,7 +14298,7 @@
         <v>847</v>
       </c>
       <c r="P184" s="25" t="s">
-        <v>898</v>
+        <v>891</v>
       </c>
       <c r="Q184" s="25"/>
       <c r="R184" s="26"/>
@@ -14327,13 +14327,13 @@
         <v>45239</v>
       </c>
       <c r="G185" s="24" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="H185" s="24" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
       <c r="I185" s="24" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="J185" s="25" t="s">
         <v>138</v>
@@ -14352,7 +14352,7 @@
         <v>847</v>
       </c>
       <c r="P185" s="25" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="Q185" s="25"/>
       <c r="R185" s="26"/>
@@ -14385,7 +14385,7 @@
         <v>847</v>
       </c>
       <c r="K186" s="25" t="s">
-        <v>905</v>
+        <v>895</v>
       </c>
       <c r="L186" s="25"/>
       <c r="M186" s="25"/>
@@ -21093,13 +21093,13 @@
         <v>45239</v>
       </c>
       <c r="G382" s="24" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="H382" s="24" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
       <c r="I382" s="24" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
       <c r="J382" s="25" t="s">
         <v>138</v>
@@ -27529,7 +27529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18989C3-D939-4409-BAFF-AA4268B3BADE}">
   <dimension ref="A1:A110"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A53" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aggiornato case test 172 come richiesto
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0349C165-96E9-45EE-8106-54C40AD4A99B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683C1B0C-75BF-4F53-ADDD-DF0F8DD53973}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4730,13 +4730,13 @@
     <t>2.16.840.1.113883.2.9.2.200.4.4.c2eff106af91871f74c0c5829c458b7a92b62b65618e9190e7193cc1cab04f04.e63c6f5804^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-01-29T15:55:45Z</t>
-  </si>
-  <si>
-    <t>240336b3e6d9300b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.200.4.4.aac6f2c803a5069fa7b90243003ff2e987782111c5b8d9f219bd595628a842a3.267f2aed2e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-01-30T17:57:57Z</t>
+  </si>
+  <si>
+    <t>0f745778d387e4f6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.200.4.4.484553b1180ba46f7b7bdd3e936906f3f740e134d26d775ff6f5c5a401e097fb.981594d4de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -7931,7 +7931,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A183" sqref="A183:XFD183"/>
+      <selection pane="bottomRight" activeCell="A179" sqref="A179:XFD179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -14036,7 +14036,7 @@
         <v>387</v>
       </c>
       <c r="F179" s="23">
-        <v>45320</v>
+        <v>45321</v>
       </c>
       <c r="G179" s="24" t="s">
         <v>903</v>

</xml_diff>

<commit_message>
aggiornamento checklist ID-46 come richiesto
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
+++ b/GATEWAY/A1#111JUNIORBIT00/SOSEPE_S.R.L/JUNIORBIT/7/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SERVIZI REGIONALI\Nazionale\FSE 2.0 2022-2026\CASE TEST PSS\v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACCREDITAMENTO GATEWAY\it-fse-accreditamento\GATEWAY\A1#111JUNIORBIT00\SOSEPE_S.R.L\JUNIORBIT\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683C1B0C-75BF-4F53-ADDD-DF0F8DD53973}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB39306-C893-457A-9495-F84BAB2C6DD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="906">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4546,9 +4546,6 @@
     <t>Messaggio errore</t>
   </si>
   <si>
-    <t>Viene mostrato un errore a video contenente il messaggio "Impossibile contattare il servizio di validazione"</t>
-  </si>
-  <si>
     <t>Essendo un elemento opzionale non viene costruito l'elemento XML.</t>
   </si>
   <si>
@@ -4668,11 +4665,6 @@
 Il test è stato effettuato per completezza e per mostrarvi l'eventuale finestra di dialogo che viene mostrata al medico in caso di errore.
 Per quanto riguarda questo specifico test non c'è possibilità da parte del medico di modificare il contenuto dei campi presenti nel token che vengono demandati completamente all'applicativo nella sua compilazione.
 In conclusione, è l'applicativo che, a priori, compila i valori del JWT e il PLS non ha nessun tipo di accesso alla sua compilazione.</t>
-  </si>
-  <si>
-    <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
-In questo caso, successivamente all'avviso a video al PLS, il retry è demandato completamente al medico.
-Non è implementata una coda di retry.</t>
   </si>
   <si>
     <t>Al PLS viene notificato il messaggio di errore bloccante, viene chiuso il processo di validazione.
@@ -4737,6 +4729,20 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.200.4.4.484553b1180ba46f7b7bdd3e936906f3f740e134d26d775ff6f5c5a401e097fb.981594d4de^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene mostrato un errore a video contenente il messaggio 
+"Impossibile contattare il servizio di validazione"
+"Il problema potrebbe essere momentaneo perciò si invita a riprovare in un secondo momento"
+"Se il problema dovesse persistere contattere l'help desk di Junior Bit."
+Ho inserito in A28 della tab "Errori interfaccia" la finestra che viene visualizzata dal medico</t>
+  </si>
+  <si>
+    <t>Al PLS viene notificato il messaggio di errore bloccante descritto nella colonna "Messaggio Errore", viene chiuso il processo di validazione.
+In questo caso, successivamente all'avviso a video al PLS, il retry è demandato completamente al medico.
+Non è implementata una coda di retry.
+Come suggerisce la finestra di dialog proposta al medico, gli viene suggerito di riprovare in un secondo momento a causa dell'impossibilità di contattare il servizio di validazione.
+Nel caso il problema dovesse persistere anche ai suoi successivi tentativi, gli viene suggerito di contattare il nostro help desk</t>
   </si>
 </sst>
 </file>
@@ -5530,6 +5536,50 @@
         <a:xfrm>
           <a:off x="0" y="15621000"/>
           <a:ext cx="7430537" cy="2000529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>103704</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Immagine 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E12EC82D-CFF8-4D17-AC70-1F13BF26A7AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5353050"/>
+          <a:ext cx="5590104" cy="2057400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7928,10 +7978,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A179" sqref="A179:XFD179"/>
+      <selection pane="bottomRight" activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7975,7 +8025,7 @@
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="42" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D2" s="41"/>
       <c r="F2" s="12"/>
@@ -9123,13 +9173,13 @@
         <v>45320</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>138</v>
@@ -9148,7 +9198,7 @@
         <v>847</v>
       </c>
       <c r="P37" s="25" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="26"/>
@@ -9415,13 +9465,13 @@
         <v>45320</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>138</v>
@@ -9440,7 +9490,7 @@
         <v>847</v>
       </c>
       <c r="P45" s="25" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
@@ -9691,7 +9741,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="14.25" customHeight="1">
+    <row r="53" spans="1:20" ht="55.5" customHeight="1">
       <c r="A53" s="20">
         <v>46</v>
       </c>
@@ -9722,13 +9772,13 @@
         <v>138</v>
       </c>
       <c r="N53" s="25" t="s">
-        <v>852</v>
+        <v>904</v>
       </c>
       <c r="O53" s="25" t="s">
         <v>847</v>
       </c>
       <c r="P53" s="25" t="s">
-        <v>889</v>
+        <v>905</v>
       </c>
       <c r="Q53" s="25"/>
       <c r="R53" s="26" t="s">
@@ -13897,7 +13947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="14.25" hidden="1" customHeight="1">
+    <row r="176" spans="1:20" ht="69" hidden="1" customHeight="1">
       <c r="A176" s="20">
         <v>169</v>
       </c>
@@ -13951,13 +14001,13 @@
         <v>45259</v>
       </c>
       <c r="G177" s="24" t="s">
+        <v>877</v>
+      </c>
+      <c r="H177" s="24" t="s">
         <v>878</v>
       </c>
-      <c r="H177" s="24" t="s">
+      <c r="I177" s="24" t="s">
         <v>879</v>
-      </c>
-      <c r="I177" s="24" t="s">
-        <v>880</v>
       </c>
       <c r="J177" s="25" t="s">
         <v>138</v>
@@ -13995,13 +14045,13 @@
         <v>45259</v>
       </c>
       <c r="G178" s="24" t="s">
+        <v>880</v>
+      </c>
+      <c r="H178" s="24" t="s">
         <v>881</v>
       </c>
-      <c r="H178" s="24" t="s">
+      <c r="I178" s="24" t="s">
         <v>882</v>
-      </c>
-      <c r="I178" s="24" t="s">
-        <v>883</v>
       </c>
       <c r="J178" s="25" t="s">
         <v>138</v>
@@ -14039,13 +14089,13 @@
         <v>45321</v>
       </c>
       <c r="G179" s="24" t="s">
+        <v>901</v>
+      </c>
+      <c r="H179" s="24" t="s">
+        <v>902</v>
+      </c>
+      <c r="I179" s="24" t="s">
         <v>903</v>
-      </c>
-      <c r="H179" s="24" t="s">
-        <v>904</v>
-      </c>
-      <c r="I179" s="24" t="s">
-        <v>905</v>
       </c>
       <c r="J179" s="25" t="s">
         <v>138</v>
@@ -14083,13 +14133,13 @@
         <v>45259</v>
       </c>
       <c r="G180" s="24" t="s">
+        <v>883</v>
+      </c>
+      <c r="H180" s="24" t="s">
         <v>884</v>
       </c>
-      <c r="H180" s="24" t="s">
+      <c r="I180" s="24" t="s">
         <v>885</v>
-      </c>
-      <c r="I180" s="24" t="s">
-        <v>886</v>
       </c>
       <c r="J180" s="25" t="s">
         <v>138</v>
@@ -14131,7 +14181,7 @@
         <v>847</v>
       </c>
       <c r="K181" s="25" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="L181" s="25"/>
       <c r="M181" s="25"/>
@@ -14165,13 +14215,13 @@
         <v>45239</v>
       </c>
       <c r="G182" s="24" t="s">
+        <v>868</v>
+      </c>
+      <c r="H182" s="24" t="s">
         <v>869</v>
       </c>
-      <c r="H182" s="24" t="s">
+      <c r="I182" s="24" t="s">
         <v>870</v>
-      </c>
-      <c r="I182" s="24" t="s">
-        <v>871</v>
       </c>
       <c r="J182" s="25" t="s">
         <v>138</v>
@@ -14190,7 +14240,7 @@
         <v>847</v>
       </c>
       <c r="P182" s="25" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="Q182" s="25"/>
       <c r="R182" s="26"/>
@@ -14219,13 +14269,13 @@
         <v>45320</v>
       </c>
       <c r="G183" s="24" t="s">
+        <v>898</v>
+      </c>
+      <c r="H183" s="24" t="s">
+        <v>899</v>
+      </c>
+      <c r="I183" s="24" t="s">
         <v>900</v>
-      </c>
-      <c r="H183" s="24" t="s">
-        <v>901</v>
-      </c>
-      <c r="I183" s="24" t="s">
-        <v>902</v>
       </c>
       <c r="J183" s="25" t="s">
         <v>138</v>
@@ -14244,7 +14294,7 @@
         <v>847</v>
       </c>
       <c r="P183" s="37" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="Q183" s="25"/>
       <c r="R183" s="26"/>
@@ -14273,13 +14323,13 @@
         <v>45239</v>
       </c>
       <c r="G184" s="24" t="s">
+        <v>871</v>
+      </c>
+      <c r="H184" s="24" t="s">
         <v>872</v>
       </c>
-      <c r="H184" s="24" t="s">
+      <c r="I184" s="24" t="s">
         <v>873</v>
-      </c>
-      <c r="I184" s="24" t="s">
-        <v>874</v>
       </c>
       <c r="J184" s="25" t="s">
         <v>138</v>
@@ -14298,7 +14348,7 @@
         <v>847</v>
       </c>
       <c r="P184" s="25" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="Q184" s="25"/>
       <c r="R184" s="26"/>
@@ -14327,13 +14377,13 @@
         <v>45239</v>
       </c>
       <c r="G185" s="24" t="s">
+        <v>874</v>
+      </c>
+      <c r="H185" s="24" t="s">
         <v>875</v>
       </c>
-      <c r="H185" s="24" t="s">
+      <c r="I185" s="24" t="s">
         <v>876</v>
-      </c>
-      <c r="I185" s="24" t="s">
-        <v>877</v>
       </c>
       <c r="J185" s="25" t="s">
         <v>138</v>
@@ -14352,7 +14402,7 @@
         <v>847</v>
       </c>
       <c r="P185" s="25" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="Q185" s="25"/>
       <c r="R185" s="26"/>
@@ -14385,7 +14435,7 @@
         <v>847</v>
       </c>
       <c r="K186" s="25" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="L186" s="25"/>
       <c r="M186" s="25"/>
@@ -14423,7 +14473,7 @@
         <v>847</v>
       </c>
       <c r="K187" s="25" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="L187" s="25"/>
       <c r="M187" s="25"/>
@@ -14461,7 +14511,7 @@
         <v>847</v>
       </c>
       <c r="K188" s="25" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="L188" s="25"/>
       <c r="M188" s="25"/>
@@ -14499,7 +14549,7 @@
         <v>847</v>
       </c>
       <c r="K189" s="25" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="L189" s="25"/>
       <c r="M189" s="25"/>
@@ -14537,7 +14587,7 @@
         <v>847</v>
       </c>
       <c r="K190" s="25" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="L190" s="25"/>
       <c r="M190" s="25"/>
@@ -14575,7 +14625,7 @@
         <v>847</v>
       </c>
       <c r="K191" s="25" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="L191" s="25"/>
       <c r="M191" s="25"/>
@@ -14613,7 +14663,7 @@
         <v>847</v>
       </c>
       <c r="K192" s="25" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="L192" s="25"/>
       <c r="M192" s="25"/>
@@ -14651,7 +14701,7 @@
         <v>847</v>
       </c>
       <c r="K193" s="25" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="L193" s="25"/>
       <c r="M193" s="25"/>
@@ -14689,7 +14739,7 @@
         <v>847</v>
       </c>
       <c r="K194" s="25" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="L194" s="25"/>
       <c r="M194" s="25"/>
@@ -14727,7 +14777,7 @@
         <v>847</v>
       </c>
       <c r="K195" s="25" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="L195" s="25"/>
       <c r="M195" s="25"/>
@@ -14765,7 +14815,7 @@
         <v>847</v>
       </c>
       <c r="K196" s="25" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="L196" s="25"/>
       <c r="M196" s="25"/>
@@ -14803,7 +14853,7 @@
         <v>847</v>
       </c>
       <c r="K197" s="25" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="L197" s="25"/>
       <c r="M197" s="25"/>
@@ -18659,7 +18709,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="14.25" customHeight="1">
+    <row r="311" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A311" s="20">
         <v>304</v>
       </c>
@@ -18693,7 +18743,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="14.25" customHeight="1">
+    <row r="312" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A312" s="20">
         <v>305</v>
       </c>
@@ -18829,7 +18879,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="14.25" customHeight="1">
+    <row r="316" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A316" s="20">
         <v>309</v>
       </c>
@@ -18863,7 +18913,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="14.25" customHeight="1">
+    <row r="317" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A317" s="20">
         <v>310</v>
       </c>
@@ -18897,7 +18947,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="14.25" customHeight="1">
+    <row r="318" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A318" s="20">
         <v>311</v>
       </c>
@@ -18931,7 +18981,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="14.25" customHeight="1">
+    <row r="319" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A319" s="20">
         <v>312</v>
       </c>
@@ -18965,7 +19015,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="14.25" customHeight="1">
+    <row r="320" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A320" s="20">
         <v>313</v>
       </c>
@@ -18999,7 +19049,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="14.25" customHeight="1">
+    <row r="321" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A321" s="20">
         <v>314</v>
       </c>
@@ -19033,7 +19083,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="14.25" customHeight="1">
+    <row r="322" spans="1:20" ht="14.25" hidden="1" customHeight="1">
       <c r="A322" s="20">
         <v>315</v>
       </c>
@@ -19135,7 +19185,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="282.75" customHeight="1">
+    <row r="325" spans="1:20" ht="282.75" hidden="1" customHeight="1">
       <c r="A325" s="20">
         <v>318</v>
       </c>
@@ -20155,7 +20205,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="242.25" customHeight="1">
+    <row r="355" spans="1:20" ht="242.25" hidden="1" customHeight="1">
       <c r="A355" s="20">
         <v>348</v>
       </c>
@@ -20189,7 +20239,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="242.25" customHeight="1">
+    <row r="356" spans="1:20" ht="242.25" hidden="1" customHeight="1">
       <c r="A356" s="20">
         <v>349</v>
       </c>
@@ -20223,7 +20273,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="315" customHeight="1">
+    <row r="357" spans="1:20" ht="315" hidden="1" customHeight="1">
       <c r="A357" s="20">
         <v>350</v>
       </c>
@@ -20257,7 +20307,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="259.5" customHeight="1">
+    <row r="358" spans="1:20" ht="259.5" hidden="1" customHeight="1">
       <c r="A358" s="20">
         <v>351</v>
       </c>
@@ -21093,13 +21143,13 @@
         <v>45239</v>
       </c>
       <c r="G382" s="24" t="s">
+        <v>865</v>
+      </c>
+      <c r="H382" s="24" t="s">
         <v>866</v>
       </c>
-      <c r="H382" s="24" t="s">
+      <c r="I382" s="24" t="s">
         <v>867</v>
-      </c>
-      <c r="I382" s="24" t="s">
-        <v>868</v>
       </c>
       <c r="J382" s="25" t="s">
         <v>138</v>
@@ -25807,6 +25857,43 @@
     <filterColumn colId="2">
       <filters>
         <filter val="PSS"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="AGGIORNAMENTO_METADATI_CDA2_PSS_CT1"/>
+        <filter val="AGGIORNAMENTO_METADATI_CDA2_PSS_CT2_KO"/>
+        <filter val="AGGIORNAMENTO_METADATI_CDA2_PSS_CT4_KO"/>
+        <filter val="AGGIORNAMENTO_METADATI_CDA2_PSS_CT5_KO"/>
+        <filter val="ELIMINAZIONE_CDA2_PSS_CT1"/>
+        <filter val="ELIMINAZIONE_CDA2_PSS_CT2_KO"/>
+        <filter val="OSCURAMENTO_CDA2_PSS_CT1"/>
+        <filter val="OSCURAMENTO_CDA2_PSS_CT2_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT0"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT1"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT10_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT11_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT12_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT13_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT14_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT15_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT16_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT17_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT18_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT19_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT2"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT20_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT21_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT3"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT4"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT5_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT6_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT7_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT8_KO"/>
+        <filter val="VALIDAZIONE_CDA2_PSS_CT9_KO"/>
+        <filter val="VALIDAZIONE_PSS_TIMEOUT"/>
+        <filter val="VALIDAZIONE_TOKEN_JWT_CAMPO_PSS_KO"/>
+        <filter val="VALIDAZIONE_TOKEN_JWT_PSS_KO"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -27529,8 +27616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18989C3-D939-4409-BAFF-AA4268B3BADE}">
   <dimension ref="A1:A110"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27546,6 +27633,11 @@
     <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:1">

</xml_diff>